<commit_message>
Admin users test case commit.
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/test/resources/TestData.xlsx
+++ b/GroceryApplication/src/test/resources/TestData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="AdminUsersPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>admin</t>
   </si>
@@ -29,6 +30,15 @@
   </si>
   <si>
     <t>admin134</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Simi</t>
+  </si>
+  <si>
+    <t>Simi123</t>
   </si>
 </sst>
 </file>
@@ -372,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -411,4 +421,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>